<commit_message>
prepare vm example spt
</commit_message>
<xml_diff>
--- a/01-deploy-synergy-from-excel/synergy.obs.hpecic.net.xlsx
+++ b/01-deploy-synergy-from-excel/synergy.obs.hpecic.net.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="11" r:id="rId1"/>
@@ -6045,7 +6045,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C7B0F21-7430-464B-906C-C94D6E6D6B12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C7B0F21-7430-464B-906C-C94D6E6D6B12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6154,7 +6154,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D0E9D9-B254-4185-8C92-46C8617F66F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01D0E9D9-B254-4185-8C92-46C8617F66F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6263,7 +6263,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D04F323B-337A-4F30-82FA-13706B020497}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D04F323B-337A-4F30-82FA-13706B020497}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10889,10 +10889,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11045,7 +11045,7 @@
         <v>508</v>
       </c>
       <c r="E17" s="4">
-        <v>1600</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -22475,7 +22475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="76" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
@@ -22483,10 +22483,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22582,8 +22582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
@@ -22755,7 +22755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
@@ -22763,8 +22763,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="76" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" style="4" customWidth="1"/>
@@ -23351,6 +23351,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B306D734CEBD84FBBC41786449802E3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16005ef843dd214786fd86ac676497e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="54a4fa2c-6341-4596-b8d8-a2e023346efc" xmlns:ns4="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2325c866b17d621340695414d4ca9b0e" ns3:_="" ns4:_="">
     <xsd:import namespace="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
@@ -23567,22 +23582,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7124AFE1-C9C5-46E7-A048-9DDD62293557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23599,29 +23624,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>